<commit_message>
fixed: when EV included, REF cost is lower than OPT cost. In the ref model, when the car is at home and being charged, it cannot be discharged. However, this is possible in the opt model.
</commit_message>
<xml_diff>
--- a/data/input_operation/OperationScenario_Component_Vehicle.xlsx
+++ b/data/input_operation/OperationScenario_Component_Vehicle.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/songminyu/Documents/Code/3E/FLEX/data/input_operation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFF80F3C-5E45-AB4F-A87B-51E8BE91B4DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBC1CCCB-EDF5-5C43-B686-B0993DD547A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-7540" yWindow="-20620" windowWidth="27600" windowHeight="18980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-640" yWindow="-20540" windowWidth="27600" windowHeight="18980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="OperationScenario_Component_Veh" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="17">
   <si>
     <t>ID_Vehicle</t>
   </si>
@@ -911,10 +911,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M11"/>
+  <dimension ref="A1:M12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -977,13 +977,13 @@
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2">
-        <v>199411</v>
+        <v>0</v>
       </c>
       <c r="B2" t="s">
         <v>13</v>
       </c>
       <c r="C2">
-        <v>69000</v>
+        <v>0</v>
       </c>
       <c r="D2" t="s">
         <v>14</v>
@@ -1018,19 +1018,19 @@
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3">
-        <v>199421</v>
+        <v>199411</v>
       </c>
       <c r="B3" t="s">
         <v>13</v>
       </c>
       <c r="C3">
-        <v>38000</v>
+        <v>69000</v>
       </c>
       <c r="D3" t="s">
         <v>14</v>
       </c>
       <c r="E3">
-        <v>153</v>
+        <v>188</v>
       </c>
       <c r="F3" t="s">
         <v>15</v>
@@ -1059,19 +1059,19 @@
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4">
-        <v>199451</v>
+        <v>199421</v>
       </c>
       <c r="B4" t="s">
         <v>13</v>
       </c>
       <c r="C4">
-        <v>69000</v>
+        <v>38000</v>
       </c>
       <c r="D4" t="s">
         <v>14</v>
       </c>
       <c r="E4">
-        <v>188</v>
+        <v>153</v>
       </c>
       <c r="F4" t="s">
         <v>15</v>
@@ -1100,19 +1100,19 @@
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5">
-        <v>199461</v>
+        <v>199451</v>
       </c>
       <c r="B5" t="s">
         <v>13</v>
       </c>
       <c r="C5">
-        <v>100000</v>
+        <v>69000</v>
       </c>
       <c r="D5" t="s">
         <v>14</v>
       </c>
       <c r="E5">
-        <v>203</v>
+        <v>188</v>
       </c>
       <c r="F5" t="s">
         <v>15</v>
@@ -1141,19 +1141,19 @@
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6">
-        <v>199462</v>
+        <v>199461</v>
       </c>
       <c r="B6" t="s">
         <v>13</v>
       </c>
       <c r="C6">
-        <v>38000</v>
+        <v>100000</v>
       </c>
       <c r="D6" t="s">
         <v>14</v>
       </c>
       <c r="E6">
-        <v>153</v>
+        <v>203</v>
       </c>
       <c r="F6" t="s">
         <v>15</v>
@@ -1182,19 +1182,19 @@
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7">
-        <v>199491</v>
+        <v>199462</v>
       </c>
       <c r="B7" t="s">
         <v>13</v>
       </c>
       <c r="C7">
-        <v>69000</v>
+        <v>38000</v>
       </c>
       <c r="D7" t="s">
         <v>14</v>
       </c>
       <c r="E7">
-        <v>188</v>
+        <v>153</v>
       </c>
       <c r="F7" t="s">
         <v>15</v>
@@ -1223,7 +1223,7 @@
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8">
-        <v>199511</v>
+        <v>199491</v>
       </c>
       <c r="B8" t="s">
         <v>13</v>
@@ -1264,19 +1264,19 @@
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9">
-        <v>199521</v>
+        <v>199511</v>
       </c>
       <c r="B9" t="s">
         <v>13</v>
       </c>
       <c r="C9">
-        <v>38000</v>
+        <v>69000</v>
       </c>
       <c r="D9" t="s">
         <v>14</v>
       </c>
       <c r="E9">
-        <v>153</v>
+        <v>188</v>
       </c>
       <c r="F9" t="s">
         <v>15</v>
@@ -1305,7 +1305,7 @@
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A10">
-        <v>199562</v>
+        <v>199521</v>
       </c>
       <c r="B10" t="s">
         <v>13</v>
@@ -1346,19 +1346,19 @@
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A11">
-        <v>1994101</v>
+        <v>199562</v>
       </c>
       <c r="B11" t="s">
         <v>13</v>
       </c>
       <c r="C11">
-        <v>100000</v>
+        <v>38000</v>
       </c>
       <c r="D11" t="s">
         <v>14</v>
       </c>
       <c r="E11">
-        <v>203</v>
+        <v>153</v>
       </c>
       <c r="F11" t="s">
         <v>15</v>
@@ -1382,6 +1382,47 @@
         <v>16</v>
       </c>
       <c r="M11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>1994101</v>
+      </c>
+      <c r="B12" t="s">
+        <v>13</v>
+      </c>
+      <c r="C12">
+        <v>100000</v>
+      </c>
+      <c r="D12" t="s">
+        <v>14</v>
+      </c>
+      <c r="E12">
+        <v>203</v>
+      </c>
+      <c r="F12" t="s">
+        <v>15</v>
+      </c>
+      <c r="G12">
+        <v>0.95</v>
+      </c>
+      <c r="H12">
+        <v>6130</v>
+      </c>
+      <c r="I12" t="s">
+        <v>16</v>
+      </c>
+      <c r="J12">
+        <v>0.9</v>
+      </c>
+      <c r="K12">
+        <v>6130</v>
+      </c>
+      <c r="L12" t="s">
+        <v>16</v>
+      </c>
+      <c r="M12">
         <v>0</v>
       </c>
     </row>

</xml_diff>